<commit_message>
bivariate prettier supp figure
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF3A802-6F4B-A24E-8582-D08C451B05D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5A603B-2791-3740-BF46-D4C117B68A84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="460" windowWidth="19220" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="126">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -368,13 +368,55 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>abridged_var_label</t>
+  </si>
+  <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Water Dist.</t>
+  </si>
+  <si>
+    <t>Urbanicity</t>
+  </si>
+  <si>
+    <t>Healthcare Dist.</t>
+  </si>
+  <si>
+    <t>Antimalarial Use</t>
+  </si>
+  <si>
+    <t>P. ovale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. falciparum </t>
+  </si>
+  <si>
+    <t>P. vivax</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>Livestock Ownership</t>
+  </si>
+  <si>
+    <t>Num. Children &lt;5</t>
+  </si>
+  <si>
+    <t>Num. House-Members</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -409,6 +451,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,7 +569,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -539,13 +589,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -621,6 +672,14 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -656,16 +715,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G52" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:G52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:G55">
-    <sortCondition ref="C1:C55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H52" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:H52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:H55">
+    <sortCondition ref="D1:D55"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="var_label"/>
+    <tableColumn id="6" xr3:uid="{1F6FE571-6C41-044D-9668-45D336EF16D5}" name="abridged_var_label" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level"/>
-    <tableColumn id="4" xr3:uid="{68699340-097D-2B4B-B268-3D5E63D9D9FA}" name="positivefactor" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{68699340-097D-2B4B-B268-3D5E63D9D9FA}" name="positivefactor" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="risk_factor_raw" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="risk_factor_model" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="iptw_model" dataDxfId="1"/>
@@ -971,24 +1031,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO52"/>
+  <dimension ref="A1:AP52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" customWidth="1"/>
-    <col min="7" max="31" width="10.83203125" style="18"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="32" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -996,23 +1057,26 @@
         <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AF1" s="18"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG1" s="18"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1020,15 +1084,18 @@
         <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="9"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="14"/>
-      <c r="AF2" s="18"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="G2" s="9"/>
+      <c r="H2" s="14"/>
+      <c r="AG2" s="18"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1036,15 +1103,18 @@
         <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="AF3" s="18"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H3" s="9"/>
+      <c r="AG3" s="18"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1052,15 +1122,18 @@
         <v>67</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="AF4" s="18"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H4" s="9"/>
+      <c r="AG4" s="18"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1068,15 +1141,18 @@
         <v>68</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="AF5" s="18"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H5" s="9"/>
+      <c r="AG5" s="18"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1084,15 +1160,18 @@
         <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="9"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="AF6" s="18"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H6" s="9"/>
+      <c r="AG6" s="18"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1100,15 +1179,18 @@
         <v>70</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="9"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="AF7" s="18"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H7" s="9"/>
+      <c r="AG7" s="18"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1116,15 +1198,18 @@
         <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="AF8" s="18"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H8" s="9"/>
+      <c r="AG8" s="18"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -1132,15 +1217,18 @@
         <v>72</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="AF9" s="18"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H9" s="9"/>
+      <c r="AG9" s="18"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
@@ -1148,15 +1236,18 @@
         <v>73</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="AF10" s="18"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H10" s="17"/>
+      <c r="AG10" s="18"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1164,17 +1255,20 @@
         <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="8"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G11" s="8"/>
-      <c r="AF11" s="18"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H11" s="8"/>
+      <c r="AG11" s="18"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1182,17 +1276,20 @@
         <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="8"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G12" s="8"/>
-      <c r="AF12" s="18"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H12" s="8"/>
+      <c r="AG12" s="18"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>85</v>
       </c>
@@ -1200,19 +1297,22 @@
         <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF13" s="18"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG13" s="18"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>86</v>
       </c>
@@ -1220,19 +1320,22 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF14" s="18"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG14" s="18"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1240,17 +1343,20 @@
         <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="8"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G15" s="8"/>
-      <c r="AF15" s="18"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H15" s="8"/>
+      <c r="AG15" s="18"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>90</v>
       </c>
@@ -1258,19 +1364,22 @@
         <v>63</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF16" s="18"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG16" s="18"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>88</v>
       </c>
@@ -1278,17 +1387,20 @@
         <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="8"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G17" s="8"/>
-      <c r="AF17" s="18"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H17" s="8"/>
+      <c r="AG17" s="18"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>87</v>
       </c>
@@ -1296,19 +1408,22 @@
         <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF18" s="18"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG18" s="18"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>97</v>
       </c>
@@ -1316,21 +1431,24 @@
         <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="8" t="s">
         <v>79</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF19" s="18"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG19" s="18"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
@@ -1338,17 +1456,20 @@
         <v>84</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="8"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G20" s="8"/>
-      <c r="AF20" s="18"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H20" s="8"/>
+      <c r="AG20" s="18"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>89</v>
       </c>
@@ -1356,19 +1477,22 @@
         <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF21" s="18"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG21" s="18"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1376,17 +1500,20 @@
         <v>96</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="8"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G22" s="8"/>
-      <c r="AF22" s="18"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H22" s="8"/>
+      <c r="AG22" s="18"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1394,81 +1521,93 @@
         <v>96</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
-        <v>79</v>
-      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AF23" s="18"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG23" s="18"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="AF24" s="18"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="G24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="AG24" s="18"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F25" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="AF25" s="18"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="G25" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="AG25" s="18"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="AF26" s="18"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H26" s="7"/>
+      <c r="AG26" s="18"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>11</v>
       </c>
@@ -1476,23 +1615,26 @@
         <v>50</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F27" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF27" s="18"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H27" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG27" s="18"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>98</v>
       </c>
@@ -1500,23 +1642,26 @@
         <v>99</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F28" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF28" s="18"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG28" s="18"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -1524,23 +1669,26 @@
         <v>51</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F29" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF29" s="18"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H29" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG29" s="18"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
@@ -1548,17 +1696,20 @@
         <v>52</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="7"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G30" s="7"/>
-      <c r="AF30" s="18"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H30" s="7"/>
+      <c r="AG30" s="18"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
@@ -1566,19 +1717,22 @@
         <v>52</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF31" s="18"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H31" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG31" s="18"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>15</v>
       </c>
@@ -1586,23 +1740,26 @@
         <v>100</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F32" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF32" s="18"/>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H32" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG32" s="18"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>91</v>
       </c>
@@ -1610,21 +1767,24 @@
         <v>53</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF33" s="18"/>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG33" s="18"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -1632,23 +1792,26 @@
         <v>54</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F34" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF34" s="18"/>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H34" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG34" s="18"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>16</v>
       </c>
@@ -1656,23 +1819,26 @@
         <v>55</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F35" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF35" s="18"/>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H35" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG35" s="18"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
@@ -1680,17 +1846,20 @@
         <v>56</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G36" s="7"/>
-      <c r="AF36" s="18"/>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H36" s="7"/>
+      <c r="AG36" s="18"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>18</v>
       </c>
@@ -1698,17 +1867,20 @@
         <v>56</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="7"/>
-      <c r="AF37" s="18"/>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="E37" s="5"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="AG37" s="18"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
@@ -1716,17 +1888,20 @@
         <v>57</v>
       </c>
       <c r="C38" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="7"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G38" s="7"/>
-      <c r="AF38" s="18"/>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H38" s="7"/>
+      <c r="AG38" s="18"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>20</v>
       </c>
@@ -1734,19 +1909,22 @@
         <v>57</v>
       </c>
       <c r="C39" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF39" s="18"/>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG39" s="18"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>94</v>
       </c>
@@ -1754,23 +1932,26 @@
         <v>95</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F40" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF40" s="18"/>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H40" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG40" s="18"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>36</v>
       </c>
@@ -1778,15 +1959,18 @@
         <v>74</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="10"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="AF41" s="18"/>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H41" s="10"/>
+      <c r="AG41" s="18"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>37</v>
       </c>
@@ -1794,15 +1978,18 @@
         <v>75</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="10"/>
+      <c r="E42" s="4"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="AF42" s="18"/>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H42" s="10"/>
+      <c r="AG42" s="18"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>38</v>
       </c>
@@ -1810,15 +1997,18 @@
         <v>38</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="10"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
-      <c r="AF43" s="18"/>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H43" s="10"/>
+      <c r="AG43" s="18"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>39</v>
       </c>
@@ -1826,15 +2016,18 @@
         <v>76</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="10"/>
+      <c r="E44" s="4"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
-      <c r="AF44" s="18"/>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H44" s="10"/>
+      <c r="AG44" s="18"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>0</v>
       </c>
@@ -1842,15 +2035,18 @@
         <v>43</v>
       </c>
       <c r="C45" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="12"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="AF45" s="18"/>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H45" s="12"/>
+      <c r="AG45" s="18"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>1</v>
       </c>
@@ -1858,15 +2054,18 @@
         <v>43</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-      <c r="AF46" s="18"/>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H46" s="12"/>
+      <c r="AG46" s="18"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>2</v>
       </c>
@@ -1874,15 +2073,18 @@
         <v>42</v>
       </c>
       <c r="C47" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="12"/>
+      <c r="E47" s="11"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
-      <c r="AF47" s="18"/>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H47" s="12"/>
+      <c r="AG47" s="18"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>3</v>
       </c>
@@ -1890,15 +2092,18 @@
         <v>42</v>
       </c>
       <c r="C48" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
-      <c r="AF48" s="18"/>
-    </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H48" s="12"/>
+      <c r="AG48" s="18"/>
+    </row>
+    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>4</v>
       </c>
@@ -1906,15 +2111,18 @@
         <v>44</v>
       </c>
       <c r="C49" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="12"/>
+      <c r="E49" s="11"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="AF49" s="18"/>
-    </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H49" s="12"/>
+      <c r="AG49" s="18"/>
+    </row>
+    <row r="50" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>5</v>
       </c>
@@ -1922,14 +2130,16 @@
         <v>44</v>
       </c>
       <c r="C50" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="12"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
-      <c r="AF50" s="18"/>
-      <c r="AG50" s="4"/>
+      <c r="H50" s="12"/>
+      <c r="AG50" s="18"/>
       <c r="AH50" s="4"/>
       <c r="AI50" s="4"/>
       <c r="AJ50" s="4"/>
@@ -1938,23 +2148,26 @@
       <c r="AM50" s="4"/>
       <c r="AN50" s="4"/>
       <c r="AO50" s="4"/>
-    </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP50" s="4"/>
+    </row>
+    <row r="51" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="12"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
-      <c r="AF51" s="18"/>
-      <c r="AG51" s="4"/>
+      <c r="H51" s="12"/>
+      <c r="AG51" s="18"/>
       <c r="AH51" s="4"/>
       <c r="AI51" s="4"/>
       <c r="AJ51" s="4"/>
@@ -1963,8 +2176,9 @@
       <c r="AM51" s="4"/>
       <c r="AN51" s="4"/>
       <c r="AO51" s="4"/>
-    </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP51" s="4"/>
+    </row>
+    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>10</v>
       </c>
@@ -1972,14 +2186,16 @@
         <v>49</v>
       </c>
       <c r="C52" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="12"/>
+      <c r="E52" s="11"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="15"/>
-      <c r="AF52" s="18"/>
-      <c r="AG52" s="4"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="15"/>
+      <c r="AG52" s="18"/>
       <c r="AH52" s="4"/>
       <c r="AI52" s="4"/>
       <c r="AJ52" s="4"/>
@@ -1988,6 +2204,7 @@
       <c r="AM52" s="4"/>
       <c r="AN52" s="4"/>
       <c r="AO52" s="4"/>
+      <c r="AP52" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sulrm covar map move
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5A603B-2791-3740-BF46-D4C117B68A84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B376D2FE-CFBF-E440-B184-E67938A9EC87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="460" windowWidth="19220" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="122">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -55,9 +55,6 @@
     <t>pfldh_fctb</t>
   </si>
   <si>
-    <t>po18s_fctb</t>
-  </si>
-  <si>
     <t>pv18s_fctb</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Falciparum infxn</t>
   </si>
   <si>
-    <t>Ovale Infxn</t>
-  </si>
-  <si>
     <t>Vivax Infxn</t>
   </si>
   <si>
@@ -346,9 +340,6 @@
     <t>falpos</t>
   </si>
   <si>
-    <t>ovpos</t>
-  </si>
-  <si>
     <t>vivpos</t>
   </si>
   <si>
@@ -389,9 +380,6 @@
   </si>
   <si>
     <t>Antimalarial Use</t>
-  </si>
-  <si>
-    <t>P. ovale</t>
   </si>
   <si>
     <t xml:space="preserve">P. falciparum </t>
@@ -598,14 +586,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -680,6 +660,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -715,20 +703,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H52" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:H52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:H55">
-    <sortCondition ref="D1:D55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:H51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:H54">
+    <sortCondition ref="D1:D54"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="var_label"/>
-    <tableColumn id="6" xr3:uid="{1F6FE571-6C41-044D-9668-45D336EF16D5}" name="abridged_var_label" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{1F6FE571-6C41-044D-9668-45D336EF16D5}" name="abridged_var_label" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level"/>
-    <tableColumn id="4" xr3:uid="{68699340-097D-2B4B-B268-3D5E63D9D9FA}" name="positivefactor" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="risk_factor_raw" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="risk_factor_model" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="iptw_model" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{68699340-097D-2B4B-B268-3D5E63D9D9FA}" name="positivefactor" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="risk_factor_raw" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="risk_factor_model" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="iptw_model" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1031,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP52"/>
+  <dimension ref="A1:AP51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:C52"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,43 +1039,43 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AG1" s="18"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="9"/>
@@ -1097,16 +1085,16 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
@@ -1116,16 +1104,16 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
@@ -1135,16 +1123,16 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="9"/>
@@ -1154,16 +1142,16 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="9"/>
@@ -1173,16 +1161,16 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="9"/>
@@ -1192,16 +1180,16 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="9"/>
@@ -1211,16 +1199,16 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="9"/>
@@ -1230,16 +1218,16 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="17"/>
@@ -1249,20 +1237,20 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1270,20 +1258,20 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1291,66 +1279,66 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG13" s="18"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG14" s="18"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1358,43 +1346,43 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1402,68 +1390,68 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -1471,43 +1459,43 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -1515,24 +1503,24 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG23" s="18"/>
     </row>
@@ -1541,22 +1529,22 @@
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H24" s="7"/>
       <c r="AG24" s="18"/>
@@ -1566,98 +1554,100 @@
         <v>7</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>121</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="AG26" s="18"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG27" s="18"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG28" s="18"/>
     </row>
@@ -1666,26 +1656,20 @@
         <v>12</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>108</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
       <c r="AG29" s="18"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
@@ -1693,20 +1677,22 @@
         <v>13</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="AG30" s="18"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
@@ -1714,48 +1700,50 @@
         <v>14</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="G31" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG31" s="18"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG32" s="18"/>
     </row>
@@ -1764,50 +1752,52 @@
         <v>91</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="F33" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG33" s="18"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG34" s="18"/>
     </row>
@@ -1816,26 +1806,20 @@
         <v>16</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>107</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
       <c r="AG35" s="18"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.2">
@@ -1843,19 +1827,19 @@
         <v>17</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="F36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="H36" s="7"/>
       <c r="AG36" s="18"/>
     </row>
@@ -1864,19 +1848,19 @@
         <v>18</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="F37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="AG37" s="18"/>
     </row>
@@ -1885,70 +1869,68 @@
         <v>19</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="AG38" s="18"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="G39" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AG39" s="18"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="A40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
       <c r="AG40" s="18"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.2">
@@ -1956,13 +1938,13 @@
         <v>36</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="10"/>
@@ -1975,13 +1957,13 @@
         <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="10"/>
@@ -1994,13 +1976,13 @@
         <v>38</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="10"/>
@@ -2009,36 +1991,36 @@
       <c r="AG43" s="18"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
+      <c r="A44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
       <c r="AG44" s="18"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="12"/>
@@ -2048,16 +2030,16 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="12"/>
@@ -2067,16 +2049,16 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="12"/>
@@ -2086,16 +2068,16 @@
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="12"/>
@@ -2105,37 +2087,46 @@
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="AG49" s="18"/>
+      <c r="AH49" s="4"/>
+      <c r="AI49" s="4"/>
+      <c r="AJ49" s="4"/>
+      <c r="AK49" s="4"/>
+      <c r="AL49" s="4"/>
+      <c r="AM49" s="4"/>
+      <c r="AN49" s="4"/>
+      <c r="AO49" s="4"/>
+      <c r="AP49" s="4"/>
     </row>
     <row r="50" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E50" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="13"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
@@ -2155,18 +2146,18 @@
         <v>9</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" s="13"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="11"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
+      <c r="H51" s="15"/>
       <c r="AG51" s="18"/>
       <c r="AH51" s="4"/>
       <c r="AI51" s="4"/>
@@ -2177,34 +2168,6 @@
       <c r="AN51" s="4"/>
       <c r="AO51" s="4"/>
       <c r="AP51" s="4"/>
-    </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="15"/>
-      <c r="AG52" s="18"/>
-      <c r="AH52" s="4"/>
-      <c r="AI52" s="4"/>
-      <c r="AJ52" s="4"/>
-      <c r="AK52" s="4"/>
-      <c r="AL52" s="4"/>
-      <c r="AM52" s="4"/>
-      <c r="AN52" s="4"/>
-      <c r="AO52" s="4"/>
-      <c r="AP52" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2226,16 +2189,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dag and null dist
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4923A73-3E8D-8542-A3C8-6EC4508088F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F605FE4-3A82-3140-AF71-CA685F08F101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19220" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="122">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t>temp_ann_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>precip</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1022,7 @@
   <dimension ref="A1:AP51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1233,7 +1239,9 @@
       <c r="A11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>103</v>
       </c>
@@ -1252,7 +1260,9 @@
       <c r="A12" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>104</v>
       </c>
@@ -1271,7 +1281,9 @@
       <c r="A13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>103</v>
       </c>
@@ -1292,7 +1304,9 @@
       <c r="A14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
URBANICITY OVERHAUL fine detaisls
just added cont clst details to variable names
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F233523E-ED78-3B47-8261-B39B8065EF7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A680E2-B1AF-F741-91E8-3B2D905C9388}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="covars" sheetId="1" r:id="rId1"/>
     <sheet name="old covars" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -482,7 +482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,6 +528,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF544D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,7 +593,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -608,6 +614,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1051,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1442,177 +1450,177 @@
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="AG20" s="18"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="AG22" s="18"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" s="8" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="21" t="s">
         <v>72</v>
       </c>
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="8" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="21" t="s">
         <v>72</v>
       </c>
       <c r="AG24" s="18"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="21" t="s">
         <v>72</v>
       </c>
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="21" t="s">
         <v>72</v>
       </c>
       <c r="AG26" s="18"/>

</xml_diff>

<commit_message>
update covar map and bivar analyss
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A680E2-B1AF-F741-91E8-3B2D905C9388}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5346629-0212-1C4E-9563-76C893C93AEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,28 +406,28 @@
     <t>Urbanicity latent variable, travel times</t>
   </si>
   <si>
-    <t>built_population_2014_scale</t>
-  </si>
-  <si>
-    <t>nightlights_composite_scale</t>
-  </si>
-  <si>
-    <t>all_population_count_2015_scale</t>
-  </si>
-  <si>
-    <t>travel_times_2015_scale</t>
-  </si>
-  <si>
-    <t>nightlights_composite</t>
-  </si>
-  <si>
-    <t>built_population_2014</t>
-  </si>
-  <si>
-    <t>all_population_count_2015</t>
-  </si>
-  <si>
-    <t>travel_times_2015</t>
+    <t>built_population_2014_cont_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nightlights_composite_cont_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all_population_count_2015_cont_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> travel_times_2015_cont_clst</t>
+  </si>
+  <si>
+    <t>built_population_2014_cont_scale_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nightlights_composite_cont_scale_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all_population_count_2015_cont_scale_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> travel_times_2015_cont_scale_clst</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:AP58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A23" sqref="A23:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>120</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>121</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>122</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>123</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>120</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>121</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>122</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
drop gaussian process from model for time for now
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5346629-0212-1C4E-9563-76C893C93AEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F95F40-6E7A-4D4D-957F-C53744897067}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="135">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -346,9 +346,6 @@
     <t>Water Dist.</t>
   </si>
   <si>
-    <t>Urbanicity</t>
-  </si>
-  <si>
     <t>Healthcare Dist.</t>
   </si>
   <si>
@@ -428,6 +425,18 @@
   </si>
   <si>
     <t xml:space="preserve"> travel_times_2015_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>Urbanicity, Nightlights</t>
+  </si>
+  <si>
+    <t>Urbanicity, Built</t>
+  </si>
+  <si>
+    <t>Urbanicity, Pop. Dens</t>
+  </si>
+  <si>
+    <t>Urbanicity, Travel Times</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1069,7 @@
   <dimension ref="A1:AP58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A26"/>
+      <selection activeCell="C23" sqref="C23:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,10 +1284,10 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>101</v>
@@ -1296,10 +1305,10 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>102</v>
@@ -1317,10 +1326,10 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>101</v>
@@ -1340,10 +1349,10 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>102</v>
@@ -1451,13 +1460,13 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>58</v>
@@ -1472,13 +1481,13 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>58</v>
@@ -1493,13 +1502,13 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>58</v>
@@ -1514,13 +1523,13 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>58</v>
@@ -1535,13 +1544,13 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>58</v>
@@ -1558,13 +1567,13 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>58</v>
@@ -1581,13 +1590,13 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>58</v>
@@ -1604,13 +1613,13 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>58</v>
@@ -1633,7 +1642,7 @@
         <v>77</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>58</v>
@@ -1654,7 +1663,7 @@
         <v>77</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>58</v>
@@ -1677,7 +1686,7 @@
         <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>58</v>
@@ -1698,7 +1707,7 @@
         <v>86</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>58</v>
@@ -1721,7 +1730,7 @@
         <v>42</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>56</v>
@@ -1746,7 +1755,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>56</v>
@@ -1767,7 +1776,7 @@
         <v>46</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>56</v>
@@ -1913,7 +1922,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>49</v>
@@ -1971,7 +1980,7 @@
         <v>51</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>56</v>
@@ -1998,7 +2007,7 @@
         <v>52</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>56</v>
@@ -2019,7 +2028,7 @@
         <v>52</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>56</v>
@@ -2040,7 +2049,7 @@
         <v>53</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>56</v>
@@ -2061,7 +2070,7 @@
         <v>53</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
make protective level the base level for factor
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391E7BDD-3882-D546-9AFE-2314796C61F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59592A05-2F9F-9449-9DE6-F5AB7A8584EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="121">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -391,13 +391,10 @@
     <t>temp</t>
   </si>
   <si>
-    <t>Urbanicity latent variable, night lights</t>
-  </si>
-  <si>
-    <t>Urbanicity, Built</t>
-  </si>
-  <si>
     <t>urbanscore_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>Urbanicity</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1027,7 @@
   <dimension ref="A1:AP51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1421,10 +1418,10 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
updates to min suff set
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -8,21 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69061674-62DA-024A-B024-6E9B323A013A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365EB037-E7F7-E64D-8063-49D74E6EEFC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="21280" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
     <sheet name="old covars" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="138">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -397,23 +402,62 @@
     <t>adjustment_set</t>
   </si>
   <si>
-    <t>"urbanscore_cont_scale_clst", "wtrdist_cont_scale_clst", "precip_ann_cont_scale_clst"</t>
-  </si>
-  <si>
-    <t>"urbanscore_cont_scale_clst", "wtrdist_cont_scale_clst", "temp_ann_cont_scale_clst"</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>urban score and water distance works</t>
+    <t>Minimally sufficient set is cluster altitude and temperature, but will include urbanicity as a potential "lurky" unknown confounder</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>conditionally independent</t>
+  </si>
+  <si>
+    <t>"urbanscore_cont_scale_clst",  "alt_dem_cont_scale_clst", "wtrdist_cont_scale_clst"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "alt_dem_cont_scale_clst", "wtrdist_cont_scale_clst"</t>
+  </si>
+  <si>
+    <t>"urbanscore_cont_scale_clst"</t>
+  </si>
+  <si>
+    <t>Going to include urbanicity which isn't necessarily needed in this min set but could be another potential confounder that I want to take into account</t>
+  </si>
+  <si>
+    <t>"hlthdist_cont_scale_clst",  "wlthrcde_fctb", "urbanscore_cont_scale_clst"</t>
+  </si>
+  <si>
+    <t>hlthdist_cont_scale_clst, wlthrcde_fctb</t>
+  </si>
+  <si>
+    <t>"urbanscore_cont_scale_clst",  "wlthrcde_fctb"</t>
+  </si>
+  <si>
+    <t>assume urban may also have a factor here -- just logistic regression works fine here</t>
+  </si>
+  <si>
+    <t>"urbanscore_cont_scale_clst",  "hv106_fctb"</t>
+  </si>
+  <si>
+    <t>"anyatm_cont_scale_clst",  "urbanscore_cont_scale_clst",  "hab57_fctb",  "hv21345_fctb",  "ITN_fctb",  "hv246_fctb", "wlthrcde_fctb"</t>
+  </si>
+  <si>
+    <t>wealth isn't needed but adding</t>
+  </si>
+  <si>
+    <t>wealth isn't needed but adding ; note wealth worked fine on own</t>
+  </si>
+  <si>
+    <t>dist health care not needed but added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,6 +500,13 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -572,7 +623,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -595,6 +646,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,6 +666,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1087,20 +1147,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="8" width="25.1640625" customWidth="1"/>
-    <col min="9" max="9" width="48.33203125" style="27" customWidth="1"/>
+    <col min="9" max="9" width="48.33203125" style="28" customWidth="1"/>
     <col min="10" max="33" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
@@ -1127,9 +1187,9 @@
         <v>74</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>120</v>
       </c>
       <c r="AH1" s="18"/>
@@ -1358,7 +1418,7 @@
       <c r="I12" s="8"/>
       <c r="AH12" s="18"/>
     </row>
-    <row r="13" spans="1:34" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>113</v>
       </c>
@@ -1376,13 +1436,15 @@
       <c r="G13" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="23" t="s">
+      <c r="H13" s="22" t="s">
         <v>122</v>
       </c>
+      <c r="I13" s="24" t="s">
+        <v>125</v>
+      </c>
       <c r="AH13" s="18"/>
     </row>
-    <row r="14" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>115</v>
       </c>
@@ -1397,15 +1459,9 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="24"/>
       <c r="AH14" s="18"/>
     </row>
     <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1448,8 +1504,12 @@
       <c r="G16" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="24"/>
+      <c r="H16" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>123</v>
+      </c>
       <c r="AH16" s="18"/>
     </row>
     <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1493,7 +1553,9 @@
         <v>72</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="24"/>
+      <c r="I18" s="25" t="s">
+        <v>123</v>
+      </c>
       <c r="AH18" s="18"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
@@ -1517,7 +1579,9 @@
         <v>72</v>
       </c>
       <c r="H19" s="21"/>
-      <c r="I19" s="25"/>
+      <c r="I19" s="26" t="s">
+        <v>126</v>
+      </c>
       <c r="AH19" s="18"/>
     </row>
     <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1561,7 +1625,9 @@
         <v>72</v>
       </c>
       <c r="H21" s="8"/>
-      <c r="I21" s="24"/>
+      <c r="I21" s="25" t="s">
+        <v>127</v>
+      </c>
       <c r="AH21" s="18"/>
     </row>
     <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1586,7 +1652,7 @@
       <c r="I22" s="8"/>
       <c r="AH22" s="18"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1604,8 +1670,12 @@
       <c r="G23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="24"/>
+      <c r="H23" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>129</v>
+      </c>
       <c r="AH23" s="18"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
@@ -1631,7 +1701,9 @@
         <v>72</v>
       </c>
       <c r="H24" s="7"/>
-      <c r="I24" s="26"/>
+      <c r="I24" s="27" t="s">
+        <v>123</v>
+      </c>
       <c r="AH24" s="18"/>
     </row>
     <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1656,7 +1728,7 @@
       <c r="I25" s="7"/>
       <c r="AH25" s="18"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
@@ -1672,14 +1744,10 @@
       <c r="E26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="26"/>
+      <c r="I26" s="27"/>
       <c r="AH26" s="18"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
@@ -1705,7 +1773,9 @@
         <v>72</v>
       </c>
       <c r="H27" s="7"/>
-      <c r="I27" s="26"/>
+      <c r="I27" s="29" t="s">
+        <v>130</v>
+      </c>
       <c r="AH27" s="18"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
@@ -1731,7 +1801,9 @@
         <v>72</v>
       </c>
       <c r="H28" s="7"/>
-      <c r="I28" s="26"/>
+      <c r="I28" s="27" t="s">
+        <v>123</v>
+      </c>
       <c r="AH28" s="18"/>
     </row>
     <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1775,10 +1847,12 @@
         <v>72</v>
       </c>
       <c r="H30" s="7"/>
-      <c r="I30" s="26"/>
+      <c r="I30" s="27" t="s">
+        <v>123</v>
+      </c>
       <c r="AH30" s="18"/>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
@@ -1800,11 +1874,15 @@
       <c r="G31" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="26"/>
+      <c r="H31" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>131</v>
+      </c>
       <c r="AH31" s="18"/>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>111</v>
       </c>
@@ -1825,10 +1903,12 @@
         <v>72</v>
       </c>
       <c r="H32" s="7"/>
-      <c r="I32" s="26"/>
+      <c r="I32" s="30" t="s">
+        <v>133</v>
+      </c>
       <c r="AH32" s="18"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>83</v>
       </c>
@@ -1851,7 +1931,9 @@
         <v>72</v>
       </c>
       <c r="H33" s="7"/>
-      <c r="I33" s="26"/>
+      <c r="I33" s="30" t="s">
+        <v>127</v>
+      </c>
       <c r="AH33" s="18"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.2">
@@ -1876,8 +1958,12 @@
       <c r="G34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="26"/>
+      <c r="H34" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>134</v>
+      </c>
       <c r="AH34" s="18"/>
     </row>
     <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1902,7 +1988,7 @@
       <c r="I35" s="7"/>
       <c r="AH35" s="18"/>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
@@ -1917,11 +2003,9 @@
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="G36" s="7"/>
       <c r="H36" s="7"/>
-      <c r="I36" s="26"/>
+      <c r="I36" s="27"/>
       <c r="AH36" s="18"/>
     </row>
     <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
@@ -1960,15 +2044,21 @@
         <v>56</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="G38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="26"/>
+      <c r="H38" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>134</v>
+      </c>
       <c r="AH38" s="18"/>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>84</v>
       </c>
@@ -1990,8 +2080,12 @@
       <c r="G39" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="26"/>
+      <c r="H39" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" s="30" t="s">
+        <v>131</v>
+      </c>
       <c r="AH39" s="18"/>
     </row>
     <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add weather data back in for lag
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365EB037-E7F7-E64D-8063-49D74E6EEFC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C2EAD9-9BF7-E845-B61E-6EA27DE97CF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="21280" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="138">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -375,27 +375,12 @@
     <t>wlthrcde_fctb</t>
   </si>
   <si>
-    <t>precip_ann_cont_clst</t>
-  </si>
-  <si>
-    <t>precip_ann_cont_scale_clst</t>
-  </si>
-  <si>
-    <t>temp_ann_cont_clst</t>
-  </si>
-  <si>
-    <t>temp_ann_cont_scale_clst</t>
-  </si>
-  <si>
     <t>precip</t>
   </si>
   <si>
     <t>temp</t>
   </si>
   <si>
-    <t>urbanscore_cont_scale_clst</t>
-  </si>
-  <si>
     <t>Urbanicity</t>
   </si>
   <si>
@@ -451,6 +436,21 @@
   </si>
   <si>
     <t>dist health care not needed but added</t>
+  </si>
+  <si>
+    <t>precip_lag_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>temp_lag_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>urban_rural_pca_fctb_clst</t>
+  </si>
+  <si>
+    <t>precip_lag_cont_clst</t>
+  </si>
+  <si>
+    <t>temp_lag_cont_clst</t>
   </si>
 </sst>
 </file>
@@ -681,6 +681,28 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -702,28 +724,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -823,13 +823,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I51" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:I51" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:I54">
     <sortCondition ref="D1:D54"/>
   </sortState>
@@ -841,8 +835,8 @@
     <tableColumn id="4" xr3:uid="{68699340-097D-2B4B-B268-3D5E63D9D9FA}" name="positivefactor" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="risk_factor_raw" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="risk_factor_model" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{615F26AB-014F-F243-BD1A-7CAA1E1BD581}" name="Notes" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="adjustment_set" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{615F26AB-014F-F243-BD1A-7CAA1E1BD581}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="adjustment_set" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1147,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,7 +1153,8 @@
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="8" width="25.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
     <col min="9" max="9" width="48.33203125" style="28" customWidth="1"/>
     <col min="10" max="33" width="10.83203125" style="18"/>
   </cols>
@@ -1187,14 +1182,14 @@
         <v>74</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AH1" s="18"/>
     </row>
-    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1214,7 +1209,7 @@
       <c r="I2" s="14"/>
       <c r="AH2" s="18"/>
     </row>
-    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1234,7 +1229,7 @@
       <c r="I3" s="9"/>
       <c r="AH3" s="18"/>
     </row>
-    <row r="4" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1254,7 +1249,7 @@
       <c r="I4" s="9"/>
       <c r="AH4" s="18"/>
     </row>
-    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1274,7 +1269,7 @@
       <c r="I5" s="9"/>
       <c r="AH5" s="18"/>
     </row>
-    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1289,7 @@
       <c r="I6" s="9"/>
       <c r="AH6" s="18"/>
     </row>
-    <row r="7" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -1314,7 +1309,7 @@
       <c r="I7" s="9"/>
       <c r="AH7" s="18"/>
     </row>
-    <row r="8" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1334,7 +1329,7 @@
       <c r="I8" s="9"/>
       <c r="AH8" s="18"/>
     </row>
-    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1354,7 +1349,7 @@
       <c r="I9" s="9"/>
       <c r="AH9" s="18"/>
     </row>
-    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>32</v>
       </c>
@@ -1374,12 +1369,12 @@
       <c r="I10" s="17"/>
       <c r="AH10" s="18"/>
     </row>
-    <row r="11" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>100</v>
@@ -1392,16 +1387,16 @@
         <v>72</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="24"/>
       <c r="AH11" s="18"/>
     </row>
-    <row r="12" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>101</v>
@@ -1410,20 +1405,18 @@
         <v>58</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="8" t="s">
-        <v>72</v>
-      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="I12" s="24"/>
       <c r="AH12" s="18"/>
     </row>
-    <row r="13" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>100</v>
@@ -1437,19 +1430,19 @@
         <v>72</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AH13" s="18"/>
     </row>
-    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>101</v>
@@ -1464,7 +1457,7 @@
       <c r="I14" s="24"/>
       <c r="AH14" s="18"/>
     </row>
-    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1505,14 +1498,14 @@
         <v>72</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AH16" s="18"/>
     </row>
-    <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>79</v>
       </c>
@@ -1554,19 +1547,19 @@
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="25" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AH18" s="18"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>58</v>
@@ -1580,11 +1573,11 @@
       </c>
       <c r="H19" s="21"/>
       <c r="I19" s="26" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AH19" s="18"/>
     </row>
-    <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
@@ -1626,11 +1619,11 @@
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="25" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AH21" s="18"/>
     </row>
-    <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1671,10 +1664,10 @@
         <v>72</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AH23" s="18"/>
     </row>
@@ -1702,11 +1695,11 @@
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AH24" s="18"/>
     </row>
-    <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>7</v>
       </c>
@@ -1728,7 +1721,7 @@
       <c r="I25" s="7"/>
       <c r="AH25" s="18"/>
     </row>
-    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
@@ -1774,7 +1767,7 @@
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="29" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="AH27" s="18"/>
     </row>
@@ -1802,11 +1795,11 @@
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AH28" s="18"/>
     </row>
-    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -1848,7 +1841,7 @@
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AH30" s="18"/>
     </row>
@@ -1875,10 +1868,10 @@
         <v>72</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AH31" s="18"/>
     </row>
@@ -1904,7 +1897,7 @@
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="AH32" s="18"/>
     </row>
@@ -1932,7 +1925,7 @@
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="30" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AH33" s="18"/>
     </row>
@@ -1959,14 +1952,14 @@
         <v>72</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I34" s="27" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AH34" s="18"/>
     </row>
-    <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>16</v>
       </c>
@@ -1988,7 +1981,7 @@
       <c r="I35" s="7"/>
       <c r="AH35" s="18"/>
     </row>
-    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
@@ -2003,12 +1996,18 @@
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="27"/>
+      <c r="G36" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>129</v>
+      </c>
       <c r="AH36" s="18"/>
     </row>
-    <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>18</v>
       </c>
@@ -2044,17 +2043,15 @@
         <v>56</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AH38" s="18"/>
     </row>
@@ -2081,14 +2078,14 @@
         <v>72</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I39" s="30" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AH39" s="18"/>
     </row>
-    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
@@ -2108,7 +2105,7 @@
       <c r="I40" s="10"/>
       <c r="AH40" s="18"/>
     </row>
-    <row r="41" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>34</v>
       </c>
@@ -2128,7 +2125,7 @@
       <c r="I41" s="10"/>
       <c r="AH41" s="18"/>
     </row>
-    <row r="42" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>35</v>
       </c>
@@ -2148,7 +2145,7 @@
       <c r="I42" s="10"/>
       <c r="AH42" s="18"/>
     </row>
-    <row r="43" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>36</v>
       </c>
@@ -2168,7 +2165,7 @@
       <c r="I43" s="10"/>
       <c r="AH43" s="18"/>
     </row>
-    <row r="44" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>0</v>
       </c>
@@ -2188,7 +2185,7 @@
       <c r="I44" s="12"/>
       <c r="AH44" s="18"/>
     </row>
-    <row r="45" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>1</v>
       </c>
@@ -2208,7 +2205,7 @@
       <c r="I45" s="12"/>
       <c r="AH45" s="18"/>
     </row>
-    <row r="46" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>2</v>
       </c>
@@ -2228,7 +2225,7 @@
       <c r="I46" s="12"/>
       <c r="AH46" s="18"/>
     </row>
-    <row r="47" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2245,7 @@
       <c r="I47" s="12"/>
       <c r="AH47" s="18"/>
     </row>
-    <row r="48" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>4</v>
       </c>
@@ -2268,7 +2265,7 @@
       <c r="I48" s="12"/>
       <c r="AH48" s="18"/>
     </row>
-    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>5</v>
       </c>
@@ -2297,7 +2294,7 @@
       <c r="AP49" s="4"/>
       <c r="AQ49" s="4"/>
     </row>
-    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>8</v>
       </c>
@@ -2326,7 +2323,7 @@
       <c r="AP50" s="4"/>
       <c r="AQ50" s="4"/>
     </row>
-    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>9</v>
       </c>
@@ -2357,6 +2354,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>